<commit_message>
updated taus spreadsheet again
</commit_message>
<xml_diff>
--- a/physical/taus.xlsx
+++ b/physical/taus.xlsx
@@ -49,6 +49,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -69,6 +70,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -113,8 +115,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -154,246 +160,246 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
+      <selection pane="topLeft" activeCell="I45" activeCellId="0" sqref="I45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>34366</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="3" t="n">
         <v>18200000000000</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <f aca="false">30</f>
         <v>30</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="4" t="n">
         <f aca="false">B2/ (4184000000000 * C2)</f>
         <v>0.144996813256851</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="2" t="n">
         <v>36174</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <f aca="false">5060000000000</f>
         <v>5060000000000</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <f aca="false">9.8</f>
         <v>9.8</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <f aca="false">B3/ (4184000000000 * C3)</f>
         <v>0.123405002536387</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="2" t="n">
         <v>38233</v>
       </c>
-      <c r="B4" s="4" t="n">
+      <c r="B4" s="5" t="n">
         <v>7260000000000</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <f aca="false">13</f>
         <v>13</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <f aca="false">B4/ (4184000000000 * C4)</f>
         <v>0.133475511104574</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="2" t="n">
         <v>38267</v>
       </c>
-      <c r="B5" s="4" t="n">
+      <c r="B5" s="5" t="n">
         <v>10400000000000</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <f aca="false">18</f>
         <v>18</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <f aca="false">B5/ (4184000000000 * C5)</f>
         <v>0.138092203101763</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="2" t="n">
         <v>39060</v>
       </c>
-      <c r="B6" s="4" t="n">
+      <c r="B6" s="5" t="n">
         <v>7410000000000</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <f aca="false">14</f>
         <v>14</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <f aca="false">B6/ (4184000000000 * C6)</f>
         <v>0.126502321770008</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="2" t="n">
         <v>40094</v>
       </c>
-      <c r="B7" s="4" t="n">
+      <c r="B7" s="5" t="n">
         <v>20000000000000</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <f aca="false">33</f>
         <v>33</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <f aca="false">B7/ (4184000000000 * C7)</f>
         <v>0.144851961295556</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="2" t="n">
         <v>40365</v>
       </c>
-      <c r="B8" s="4" t="n">
+      <c r="B8" s="5" t="n">
         <v>7560000000000</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <f aca="false">14</f>
         <v>14</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <f aca="false">B8/ (4184000000000 * C8)</f>
         <v>0.12906309751434</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="2" t="n">
         <v>40537</v>
       </c>
-      <c r="B9" s="4" t="n">
+      <c r="B9" s="5" t="n">
         <v>20000000000000</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <f aca="false">33</f>
         <v>33</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <f aca="false">B9/ (4184000000000 * C9)</f>
         <v>0.144851961295556</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+      <c r="A10" s="2" t="n">
         <v>41320</v>
       </c>
-      <c r="B10" s="4" t="n">
+      <c r="B10" s="5" t="n">
         <v>375000000000000</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <f aca="false">440</f>
         <v>440</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <f aca="false">B10/ (4184000000000 * C10)</f>
         <v>0.203698070571876</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+      <c r="A11" s="2" t="n">
         <v>41394</v>
       </c>
-      <c r="B11" s="4" t="n">
+      <c r="B11" s="5" t="n">
         <v>5110000000000</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <f aca="false">10</f>
         <v>10</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <f aca="false">B11/ (4184000000000 * C11)</f>
         <v>0.122131931166348</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+      <c r="A12" s="2" t="n">
         <v>42406</v>
       </c>
-      <c r="B12" s="4" t="n">
+      <c r="B12" s="5" t="n">
         <v>6853000000000</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <f aca="false">13</f>
         <v>13</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <f aca="false">B12/ (4184000000000 * C12)</f>
         <v>0.125992793057803</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+      <c r="A13" s="2" t="n">
         <v>43452</v>
       </c>
-      <c r="B13" s="4" t="n">
+      <c r="B13" s="5" t="n">
         <v>31300000000000</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <f aca="false">49</f>
         <v>49</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <f aca="false">B13/ (4184000000000 * C13)</f>
         <v>0.152671011043041</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+      <c r="A14" s="2" t="n">
         <v>44187</v>
       </c>
-      <c r="B14" s="4" t="n">
+      <c r="B14" s="5" t="n">
         <v>4898000000000</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <f aca="false">9.5</f>
         <v>9.5</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <f aca="false">B14/ (4184000000000 * C14)</f>
         <v>0.123226325852873</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+      <c r="A15" s="2" t="n">
         <v>44599</v>
       </c>
-      <c r="B15" s="4" t="n">
+      <c r="B15" s="5" t="n">
         <v>3480000000000</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <f aca="false">7</f>
         <v>7</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <f aca="false">B15/ (4184000000000 * C15)</f>
         <v>0.118819994537012</v>
       </c>

</xml_diff>

<commit_message>
updated taus excel spreadsheet and csv to have kosice, romania, flensburg and almahatta sitta taus empirically computed from the values given on CNEOS website
</commit_message>
<xml_diff>
--- a/physical/taus.xlsx
+++ b/physical/taus.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">event</t>
   </si>
@@ -32,6 +32,18 @@
   </si>
   <si>
     <t xml:space="preserve">tau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kosice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">romania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flensburg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">almahatta sitta</t>
   </si>
 </sst>
 </file>
@@ -115,7 +127,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -138,6 +150,10 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -157,13 +173,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I45" activeCellId="0" sqref="I45"/>
+      <selection pane="topLeft" activeCell="L34" activeCellId="0" sqref="L34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -402,6 +418,66 @@
       <c r="D15" s="1" t="n">
         <f aca="false">B15/ (4184000000000 * C15)</f>
         <v>0.118819994537012</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="6" t="n">
+        <v>153000000000</v>
+      </c>
+      <c r="C16" s="6" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <f aca="false">B16/ (4184000000000 * C16)</f>
+        <v>0.0831088127933252</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="6" t="n">
+        <v>136000000000</v>
+      </c>
+      <c r="C17" s="6" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <f aca="false">B17/ (4184000000000 * C17)</f>
+        <v>0.0812619502868069</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="6" t="n">
+        <v>169000000000</v>
+      </c>
+      <c r="C18" s="6" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <f aca="false">B18/ (4184000000000 * C18)</f>
+        <v>0.084149936265137</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="6" t="n">
+        <v>395000000000</v>
+      </c>
+      <c r="C19" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <f aca="false">B19/ (4184000000000 * C19)</f>
+        <v>0.0944072657743786</v>
       </c>
     </row>
   </sheetData>

</xml_diff>